<commit_message>
Text changes to support the tech changes
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CEQ-topic.xlsx
+++ b/output/StructureDefinition-CEQ-topic.xlsx
@@ -2569,10 +2569,10 @@
       </c>
       <c r="P18" s="2"/>
       <c r="Q18" t="s" s="2">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="R18" t="s" s="2">
-        <v>142</v>
+        <v>41</v>
       </c>
       <c r="S18" t="s" s="2">
         <v>41</v>

</xml_diff>